<commit_message>
updated by county landfall probabilies in xls spreadsheet - BH
</commit_message>
<xml_diff>
--- a/Project -BH/landfall_probabilities.xlsx
+++ b/Project -BH/landfall_probabilities.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12038\Desktop\Project 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12038\Project-1-\Project -BH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{83161E0F-B57E-4E91-9E94-27C1555DF492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163E06DA-E313-4B12-B9BA-1B561040CC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="260" windowWidth="15890" windowHeight="7560"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="landfall_probabilities" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">landfall_probabilities!$A$1:$K$113</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$3:$U$53</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="194">
   <si>
     <t>State</t>
   </si>
@@ -566,17 +567,60 @@
   </si>
   <si>
     <t>50 Year Probability of Intense Hurricane-Force (&gt;= 115 mph) Wind Gusts in the County</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>Gadsden</t>
+  </si>
+  <si>
+    <t>Gilchrist</t>
+  </si>
+  <si>
+    <t>Hillsborough</t>
+  </si>
+  <si>
+    <t>Holmes</t>
+  </si>
+  <si>
+    <t>Lafayette</t>
+  </si>
+  <si>
+    <t>Leon</t>
+  </si>
+  <si>
+    <t>Madison</t>
+  </si>
+  <si>
+    <t>Okeechobee</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Osceola</t>
+  </si>
+  <si>
+    <t>Putnam</t>
+  </si>
+  <si>
+    <t>Seminole</t>
+  </si>
+  <si>
+    <t>St Lucie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -728,11 +772,15 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Calibri  "/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri  "/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -912,6 +960,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1075,7 +1129,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1092,14 +1146,18 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="10" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="21" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="169" fontId="20" fillId="33" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="21" fillId="33" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="20" fillId="33" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -1505,24 +1563,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="11.90625" customWidth="1"/>
     <col min="3" max="3" width="18.6328125" customWidth="1"/>
     <col min="4" max="4" width="14.26953125" customWidth="1"/>
-    <col min="11" max="11" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="13.81640625" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="18.08984375" customWidth="1"/>
     <col min="13" max="13" width="8.7265625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1557,7 +1620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1592,7 +1655,7 @@
         <v>7.0000000000000009</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1627,7 +1690,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1662,7 +1725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1697,7 +1760,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1732,7 +1795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1767,7 +1830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1802,7 +1865,7 @@
         <v>7.0000000000000009</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1837,7 +1900,7 @@
         <v>7.0000000000000009</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1872,7 +1935,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1907,7 +1970,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1942,7 +2005,7 @@
         <v>7.0000000000000009</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1977,7 +2040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -2012,7 +2075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -2047,7 +2110,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -2082,7 +2145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -2117,7 +2180,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2152,7 +2215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -2187,7 +2250,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -2222,7 +2285,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -2257,7 +2320,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -2292,7 +2355,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -2327,7 +2390,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -2362,7 +2425,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -2397,7 +2460,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -2432,7 +2495,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -2467,7 +2530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -2502,7 +2565,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -2537,7 +2600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2572,7 +2635,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -2607,7 +2670,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -2642,7 +2705,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -2677,7 +2740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -2712,7 +2775,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -2747,7 +2810,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -2782,7 +2845,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2817,7 +2880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -2852,7 +2915,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -2887,7 +2950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -2922,7 +2985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2957,7 +3020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2992,7 +3055,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -3027,7 +3090,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -3062,7 +3125,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -3097,7 +3160,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>41</v>
       </c>
@@ -3132,7 +3195,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -3167,7 +3230,7 @@
         <v>14.000000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -3202,7 +3265,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11">
       <c r="A49" t="s">
         <v>41</v>
       </c>
@@ -3237,7 +3300,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
         <v>41</v>
       </c>
@@ -3272,7 +3335,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>41</v>
       </c>
@@ -3307,7 +3370,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
         <v>41</v>
       </c>
@@ -3342,7 +3405,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>41</v>
       </c>
@@ -3377,7 +3440,7 @@
         <v>14.000000000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11">
       <c r="A54" t="s">
         <v>41</v>
       </c>
@@ -3412,7 +3475,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11">
       <c r="A55" t="s">
         <v>41</v>
       </c>
@@ -3447,7 +3510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11">
       <c r="A56" t="s">
         <v>41</v>
       </c>
@@ -3482,7 +3545,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11">
       <c r="A57" t="s">
         <v>41</v>
       </c>
@@ -3517,7 +3580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11">
       <c r="A58" t="s">
         <v>41</v>
       </c>
@@ -3552,7 +3615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11">
       <c r="A59" t="s">
         <v>41</v>
       </c>
@@ -3587,7 +3650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11">
       <c r="A60" t="s">
         <v>41</v>
       </c>
@@ -3622,7 +3685,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11">
       <c r="A61" t="s">
         <v>41</v>
       </c>
@@ -3657,7 +3720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11">
       <c r="A62" t="s">
         <v>41</v>
       </c>
@@ -3692,7 +3755,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -3727,7 +3790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11">
       <c r="A64" t="s">
         <v>75</v>
       </c>
@@ -3762,7 +3825,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11">
       <c r="A65" t="s">
         <v>75</v>
       </c>
@@ -3797,7 +3860,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11">
       <c r="A66" t="s">
         <v>75</v>
       </c>
@@ -3832,7 +3895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -3867,7 +3930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -3902,7 +3965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11">
       <c r="A69" t="s">
         <v>82</v>
       </c>
@@ -3937,7 +4000,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -3972,7 +4035,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -4007,7 +4070,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11">
       <c r="A72" t="s">
         <v>82</v>
       </c>
@@ -4042,7 +4105,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11">
       <c r="A73" t="s">
         <v>82</v>
       </c>
@@ -4077,7 +4140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -4112,7 +4175,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11">
       <c r="A75" t="s">
         <v>89</v>
       </c>
@@ -4147,7 +4210,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11">
       <c r="A76" t="s">
         <v>89</v>
       </c>
@@ -4182,7 +4245,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11">
       <c r="A77" t="s">
         <v>89</v>
       </c>
@@ -4217,7 +4280,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11">
       <c r="A78" t="s">
         <v>89</v>
       </c>
@@ -4252,7 +4315,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11">
       <c r="A79" t="s">
         <v>89</v>
       </c>
@@ -4287,7 +4350,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11">
       <c r="A80" t="s">
         <v>89</v>
       </c>
@@ -4322,7 +4385,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11">
       <c r="A81" t="s">
         <v>89</v>
       </c>
@@ -4357,7 +4420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11">
       <c r="A82" t="s">
         <v>89</v>
       </c>
@@ -4392,7 +4455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11">
       <c r="A83" t="s">
         <v>98</v>
       </c>
@@ -4427,7 +4490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11">
       <c r="A84" t="s">
         <v>98</v>
       </c>
@@ -4462,7 +4525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11">
       <c r="A85" t="s">
         <v>98</v>
       </c>
@@ -4497,7 +4560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11">
       <c r="A86" t="s">
         <v>102</v>
       </c>
@@ -4532,7 +4595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11">
       <c r="A87" t="s">
         <v>104</v>
       </c>
@@ -4567,7 +4630,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11">
       <c r="A88" t="s">
         <v>107</v>
       </c>
@@ -4602,7 +4665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11">
       <c r="A89" t="s">
         <v>107</v>
       </c>
@@ -4637,7 +4700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11">
       <c r="A90" t="s">
         <v>107</v>
       </c>
@@ -4672,7 +4735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11">
       <c r="A91" t="s">
         <v>107</v>
       </c>
@@ -4707,7 +4770,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11">
       <c r="A92" t="s">
         <v>112</v>
       </c>
@@ -4742,7 +4805,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11">
       <c r="A93" t="s">
         <v>112</v>
       </c>
@@ -4777,7 +4840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11">
       <c r="A94" t="s">
         <v>112</v>
       </c>
@@ -4812,7 +4875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11">
       <c r="A95" t="s">
         <v>112</v>
       </c>
@@ -4847,7 +4910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11">
       <c r="A96" t="s">
         <v>116</v>
       </c>
@@ -4882,7 +4945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11">
       <c r="A97" t="s">
         <v>116</v>
       </c>
@@ -4917,7 +4980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11">
       <c r="A98" t="s">
         <v>116</v>
       </c>
@@ -4952,7 +5015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11">
       <c r="A99" t="s">
         <v>120</v>
       </c>
@@ -4987,7 +5050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11">
       <c r="A100" t="s">
         <v>120</v>
       </c>
@@ -5022,7 +5085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11">
       <c r="A101" t="s">
         <v>120</v>
       </c>
@@ -5057,7 +5120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11">
       <c r="A102" t="s">
         <v>120</v>
       </c>
@@ -5092,7 +5155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11">
       <c r="A103" t="s">
         <v>120</v>
       </c>
@@ -5127,7 +5190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11">
       <c r="A104" t="s">
         <v>120</v>
       </c>
@@ -5162,7 +5225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11">
       <c r="A105" t="s">
         <v>120</v>
       </c>
@@ -5197,7 +5260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11">
       <c r="A106" t="s">
         <v>127</v>
       </c>
@@ -5232,7 +5295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11">
       <c r="A107" t="s">
         <v>129</v>
       </c>
@@ -5267,7 +5330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11">
       <c r="A108" t="s">
         <v>129</v>
       </c>
@@ -5302,7 +5365,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11">
       <c r="A109" t="s">
         <v>129</v>
       </c>
@@ -5337,7 +5400,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11">
       <c r="A110" t="s">
         <v>129</v>
       </c>
@@ -5372,7 +5435,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11">
       <c r="A111" t="s">
         <v>129</v>
       </c>
@@ -5407,7 +5470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11">
       <c r="A112" t="s">
         <v>129</v>
       </c>
@@ -5442,7 +5505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:11">
       <c r="A113" t="s">
         <v>129</v>
       </c>
@@ -5478,43 +5541,37 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K113">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Florida"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K113" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="24.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="24.7265625" style="2"/>
     <col min="2" max="2" width="24.7265625" style="3"/>
     <col min="3" max="16384" width="24.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3">
       <c r="B1" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" ht="15.5">
       <c r="B2" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3">
       <c r="B4" s="6" t="s">
         <v>138</v>
       </c>
@@ -5522,7 +5579,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3">
       <c r="B5" s="3" t="s">
         <v>140</v>
       </c>
@@ -5530,7 +5587,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3">
       <c r="B6" s="3" t="s">
         <v>142</v>
       </c>
@@ -5538,7 +5595,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3">
       <c r="B7" s="3" t="s">
         <v>149</v>
       </c>
@@ -5546,7 +5603,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3">
       <c r="B8" s="3" t="s">
         <v>150</v>
       </c>
@@ -5554,7 +5611,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3">
       <c r="B9" s="3" t="s">
         <v>151</v>
       </c>
@@ -5562,7 +5619,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3">
       <c r="B10" s="3" t="s">
         <v>152</v>
       </c>
@@ -5570,7 +5627,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3">
       <c r="B11" s="3" t="s">
         <v>153</v>
       </c>
@@ -5578,7 +5635,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3">
       <c r="B12" s="3" t="s">
         <v>154</v>
       </c>
@@ -5593,204 +5650,3452 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:U1048575"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="2" width="8.7265625" style="9"/>
+    <col min="3" max="3" width="8.7265625" style="15"/>
+    <col min="4" max="4" width="29.36328125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="24" style="9" customWidth="1"/>
+    <col min="6" max="6" width="30.36328125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.453125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="21" style="9" customWidth="1"/>
+    <col min="9" max="9" width="20.08984375" style="9" customWidth="1"/>
+    <col min="10" max="10" width="21.1796875" style="9" customWidth="1"/>
+    <col min="11" max="11" width="16.6328125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="19.36328125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="21" style="9" customWidth="1"/>
+    <col min="14" max="14" width="15.08984375" style="9" customWidth="1"/>
+    <col min="15" max="15" width="16.90625" style="9" customWidth="1"/>
+    <col min="16" max="16" width="18.08984375" style="9" customWidth="1"/>
+    <col min="17" max="17" width="14.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.90625" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.7265625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="12"/>
+      <c r="D2" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="88.5" customHeight="1">
+      <c r="A3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="15">
+        <v>4</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F4" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G4" s="12">
+        <v>0.104</v>
+      </c>
+      <c r="H4" s="12">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="I4" s="12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J4" s="12">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0.113</v>
+      </c>
+      <c r="L4" s="12">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O4" s="11">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P4" s="12">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>0.73</v>
+      </c>
+      <c r="R4" s="12">
+        <v>0.127</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T4" s="12">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U4" s="12">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="15">
+        <v>7</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="F5" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G5" s="9">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="H5" s="9">
+        <v>3.1E-2</v>
+      </c>
+      <c r="I5" s="9">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="K5" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L5" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N5" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O5" s="13">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="P5" s="9">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="R5" s="9">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="S5" s="9">
+        <v>0.995</v>
+      </c>
+      <c r="T5" s="9">
+        <v>0.746</v>
+      </c>
+      <c r="U5" s="9">
+        <v>0.39500000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="15">
+        <v>6</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="G6" s="9">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H6" s="9">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="I6" s="9">
+        <v>2.3E-2</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="L6" s="9">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="P6" s="9">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>0.747</v>
+      </c>
+      <c r="R6" s="9">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="S6" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T6" s="9">
+        <v>0.999</v>
+      </c>
+      <c r="U6" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="15">
+        <v>4</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F7" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G7" s="9">
+        <v>3.1E-2</v>
+      </c>
+      <c r="H7" s="9">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I7" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="L7" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O7" s="13">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P7" s="9">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="R7" s="9">
+        <v>0.308</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T7" s="9">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U7" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="15">
+        <v>5</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F8" s="13">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="I8" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J8" s="9">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="K8" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="L8" s="9">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N8" s="13">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="O8" s="13">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="P8" s="9">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>0.246</v>
+      </c>
+      <c r="R8" s="9">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="S8" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T8" s="9">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="U8" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="15">
+        <v>4</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F9" s="13">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G9" s="9">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H9" s="9">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="I9" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K9" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="L9" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O9" s="13">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P9" s="9">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="R9" s="9">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="S9" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T9" s="9">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U9" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" s="15">
+        <v>7</v>
+      </c>
+      <c r="D10" s="13">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="F10" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G10" s="9">
+        <v>1.9E-2</v>
+      </c>
+      <c r="H10" s="9">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I10" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="J10" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="K10" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L10" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N10" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O10" s="13">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="P10" s="9">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="Q10" s="9">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="R10" s="9">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="S10" s="9">
+        <v>0.995</v>
+      </c>
+      <c r="T10" s="9">
+        <v>0.746</v>
+      </c>
+      <c r="U10" s="9">
+        <v>0.39500000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="15">
+        <v>5</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F11" s="13">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="G11" s="9">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="H11" s="9">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="I11" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="J11" s="9">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="K11" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="L11" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N11" s="13">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="O11" s="13">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="P11" s="9">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="Q11" s="9">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="R11" s="9">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="S11" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T11" s="9">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="U11" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="15">
+        <v>4</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F12" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G12" s="12">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H12" s="12">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="I12" s="12">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K12" s="12">
+        <v>0.113</v>
+      </c>
+      <c r="L12" s="12">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O12" s="11">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P12" s="12">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="Q12" s="12">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="R12" s="12">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="S12" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T12" s="12">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U12" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="15">
+        <v>7</v>
+      </c>
+      <c r="D13" s="13">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="E13" s="13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="F13" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="H13" s="9">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I13" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="K13" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L13" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M13" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N13" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O13" s="13">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="P13" s="9">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="Q13" s="9">
+        <v>0.215</v>
+      </c>
+      <c r="R13" s="9">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="S13" s="9">
+        <v>0.995</v>
+      </c>
+      <c r="T13" s="9">
+        <v>0.746</v>
+      </c>
+      <c r="U13" s="9">
+        <v>0.39500000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="15">
+        <v>3</v>
+      </c>
+      <c r="D14" s="13">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="G14" s="9">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="H14" s="9">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="I14" s="9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="J14" s="9">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="K14" s="9">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="L14" s="9">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="M14" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N14" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O14" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="P14" s="9">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="Q14" s="9">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="R14" s="9">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="S14" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T14" s="9">
+        <v>0.996</v>
+      </c>
+      <c r="U14" s="9">
+        <v>0.82299999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="15">
+        <v>7</v>
+      </c>
+      <c r="D15" s="13">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="F15" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G15" s="9">
+        <v>1.9E-2</v>
+      </c>
+      <c r="H15" s="9">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I15" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="K15" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L15" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N15" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O15" s="13">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="P15" s="9">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="Q15" s="9">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="R15" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="S15" s="9">
+        <v>0.995</v>
+      </c>
+      <c r="T15" s="9">
+        <v>0.746</v>
+      </c>
+      <c r="U15" s="9">
+        <v>0.39500000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="15">
+        <v>4</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F16" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G16" s="9">
+        <v>0.11</v>
+      </c>
+      <c r="H16" s="9">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="I16" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K16" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="L16" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N16" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O16" s="13">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P16" s="9">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="Q16" s="9">
+        <v>0.751</v>
+      </c>
+      <c r="R16" s="9">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="S16" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T16" s="9">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U16" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C17" s="15">
+        <v>4</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F17" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G17" s="9">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="H17" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="I17" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K17" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="L17" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M17" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O17" s="13">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P17" s="9">
+        <v>0.72</v>
+      </c>
+      <c r="Q17" s="9">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="R17" s="9">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="S17" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T17" s="9">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U17" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
+      <c r="A18" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18" s="15">
+        <v>4</v>
+      </c>
+      <c r="D18" s="11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E18" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F18" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G18" s="9">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H18" s="9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="I18" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="J18" s="9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K18" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="L18" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M18" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O18" s="13">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P18" s="9">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="R18" s="9">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="S18" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T18" s="9">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U18" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="15">
+        <v>4</v>
+      </c>
+      <c r="D19" s="11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E19" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F19" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G19" s="9">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="H19" s="9">
+        <v>1.9E-2</v>
+      </c>
+      <c r="I19" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K19" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="L19" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M19" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N19" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O19" s="13">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P19" s="9">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="R19" s="9">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="S19" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T19" s="9">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U19" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="15">
+        <v>5</v>
+      </c>
+      <c r="D20" s="13">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E20" s="13">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F20" s="13">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="G20" s="9">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H20" s="9">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="I20" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J20" s="9">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="K20" s="9">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="L20" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M20" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N20" s="13">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="O20" s="13">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="P20" s="9">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="Q20" s="9">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="R20" s="9">
+        <v>0.156</v>
+      </c>
+      <c r="S20" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T20" s="9">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="U20" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" s="15">
+        <v>5</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F21" s="13">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="G21" s="9">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="H21" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="K21" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="L21" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M21" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N21" s="13">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="O21" s="13">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="P21" s="9">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="Q21" s="9">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="R21" s="9">
+        <v>0.246</v>
+      </c>
+      <c r="S21" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T21" s="9">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="U21" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="A22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C22" s="15">
+        <v>3</v>
+      </c>
+      <c r="D22" s="13">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="E22" s="13">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="F22" s="13">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="G22" s="9">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H22" s="9">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I22" s="9">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J22" s="9">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="K22" s="9">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="L22" s="9">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N22" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O22" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="P22" s="9">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="Q22" s="9">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="R22" s="9">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="S22" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T22" s="9">
+        <v>0.996</v>
+      </c>
+      <c r="U22" s="9">
+        <v>0.82299999999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="A23" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="15">
+        <v>7</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="F23" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G23" s="9">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="H23" s="9">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I23" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="K23" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L23" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N23" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O23" s="13">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="P23" s="9">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="Q23" s="9">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="R23" s="9">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="S23" s="9">
+        <v>0.995</v>
+      </c>
+      <c r="T23" s="9">
+        <v>0.746</v>
+      </c>
+      <c r="U23" s="9">
+        <v>0.39500000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="A24" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="15">
+        <v>4</v>
+      </c>
+      <c r="D24" s="11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E24" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F24" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G24" s="9">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="H24" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I24" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="J24" s="9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K24" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="L24" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M24" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N24" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O24" s="13">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P24" s="9">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="Q24" s="9">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="R24" s="9">
+        <v>1.6E-2</v>
+      </c>
+      <c r="S24" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T24" s="9">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U24" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="A25" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" s="15">
+        <v>4</v>
+      </c>
+      <c r="D25" s="11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E25" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F25" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G25" s="9">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="H25" s="9">
+        <v>2.7E-2</v>
+      </c>
+      <c r="I25" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K25" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="L25" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M25" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N25" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O25" s="13">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P25" s="9">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="Q25" s="9">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="R25" s="9">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="S25" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T25" s="9">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U25" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="A26" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="15">
+        <v>5</v>
+      </c>
+      <c r="D26" s="13">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E26" s="13">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F26" s="13">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="G26" s="9">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="H26" s="9">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="I26" s="9">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J26" s="9">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="K26" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="L26" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M26" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N26" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O26" s="13">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="P26" s="9">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="Q26" s="9">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="R26" s="9">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="S26" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T26" s="9">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="U26" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C27" s="15">
+        <v>4</v>
+      </c>
+      <c r="D27" s="11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E27" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F27" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G27" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H27" s="9">
+        <v>3.1E-2</v>
+      </c>
+      <c r="I27" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K27" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="L27" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M27" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N27" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O27" s="13">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P27" s="9">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="Q27" s="9">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="R27" s="9">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="S27" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T27" s="9">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U27" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="15">
+        <v>4</v>
+      </c>
+      <c r="D28" s="11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E28" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F28" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G28" s="9">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="H28" s="9">
+        <v>3.1E-2</v>
+      </c>
+      <c r="I28" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J28" s="9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K28" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="L28" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M28" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N28" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O28" s="13">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P28" s="9">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="Q28" s="9">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="R28" s="9">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="S28" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T28" s="9">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U28" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="15">
+        <v>4</v>
+      </c>
+      <c r="D29" s="11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E29" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F29" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G29" s="9">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="H29" s="9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I29" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K29" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="L29" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M29" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N29" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O29" s="13">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P29" s="9">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="Q29" s="9">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="R29" s="9">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="S29" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T29" s="9">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U29" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="A30" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C30" s="15">
+        <v>4</v>
+      </c>
+      <c r="D30" s="11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E30" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F30" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G30" s="9">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="H30" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="I30" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J30" s="9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K30" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="L30" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O30" s="13">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P30" s="9">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="Q30" s="9">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="R30" s="9">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="S30" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T30" s="9">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U30" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="A31" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="15">
+        <v>5</v>
+      </c>
+      <c r="D31" s="13">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E31" s="13">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F31" s="13">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="G31" s="9">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H31" s="9">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I31" s="9">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J31" s="9">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="K31" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="L31" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M31" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N31" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O31" s="13">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="P31" s="9">
+        <v>0.627</v>
+      </c>
+      <c r="Q31" s="9">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="R31" s="9">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="S31" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T31" s="9">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="U31" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="15">
+        <v>6</v>
+      </c>
+      <c r="D32" s="13">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="E32" s="13">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="F32" s="13">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="G32" s="9">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="H32" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="I32" s="9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="J32" s="9">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="K32" s="9">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="L32" s="9">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="M32" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N32" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O32" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="P32" s="9">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="Q32" s="9">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="R32" s="9">
+        <v>0.311</v>
+      </c>
+      <c r="S32" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T32" s="9">
+        <v>0.999</v>
+      </c>
+      <c r="U32" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
+      <c r="A33" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="15">
+        <v>6</v>
+      </c>
+      <c r="D33" s="13">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="E33" s="13">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="F33" s="13">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="H33" s="9">
+        <v>0.105</v>
+      </c>
+      <c r="I33" s="9">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="J33" s="9">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="K33" s="9">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="L33" s="9">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="M33" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N33" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O33" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="P33" s="9">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="Q33" s="9">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="R33" s="9">
+        <v>0.753</v>
+      </c>
+      <c r="S33" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T33" s="9">
+        <v>0.999</v>
+      </c>
+      <c r="U33" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
+      <c r="A34" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="15">
+        <v>6</v>
+      </c>
+      <c r="D34" s="13">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="E34" s="13">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="F34" s="13">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="G34" s="9">
+        <v>0.371</v>
+      </c>
+      <c r="H34" s="9">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="I34" s="9">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="J34" s="9">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="K34" s="9">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="L34" s="9">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="M34" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N34" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O34" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="P34" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q34" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="R34" s="9">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="S34" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T34" s="9">
+        <v>0.999</v>
+      </c>
+      <c r="U34" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
+      <c r="A35" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="15">
+        <v>7</v>
+      </c>
+      <c r="D35" s="13">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="E35" s="13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="F35" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G35" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="H35" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I35" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="J35" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="K35" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L35" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M35" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N35" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O35" s="13">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="P35" s="9">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="Q35" s="9">
+        <v>0.114</v>
+      </c>
+      <c r="R35" s="9">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="S35" s="9">
+        <v>0.995</v>
+      </c>
+      <c r="T35" s="9">
+        <v>0.746</v>
+      </c>
+      <c r="U35" s="9">
+        <v>0.39500000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
+      <c r="A36" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="15">
+        <v>3</v>
+      </c>
+      <c r="D36" s="13">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="E36" s="13">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="F36" s="13">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="G36" s="9">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="H36" s="9">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="I36" s="9">
+        <v>1.9E-2</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="K36" s="9">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="L36" s="9">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="M36" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N36" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O36" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="P36" s="9">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="Q36" s="9">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="R36" s="9">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="S36" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T36" s="9">
+        <v>0.996</v>
+      </c>
+      <c r="U36" s="9">
+        <v>0.82299999999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
+      <c r="A37" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C37" s="15">
+        <v>7</v>
+      </c>
+      <c r="D37" s="13">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="E37" s="13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="F37" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G37" s="9">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="H37" s="9">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="I37" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J37" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="K37" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L37" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M37" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N37" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O37" s="13">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="P37" s="9">
+        <v>0.51</v>
+      </c>
+      <c r="Q37" s="9">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="R37" s="9">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="S37" s="9">
+        <v>0.995</v>
+      </c>
+      <c r="T37" s="9">
+        <v>0.746</v>
+      </c>
+      <c r="U37" s="9">
+        <v>0.39500000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
+      <c r="A38" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C38" s="15">
+        <v>7</v>
+      </c>
+      <c r="D38" s="13">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="E38" s="13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="F38" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G38" s="9">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H38" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I38" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="J38" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="K38" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L38" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M38" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N38" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O38" s="13">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="P38" s="9">
+        <v>0.33</v>
+      </c>
+      <c r="Q38" s="9">
+        <v>0.161</v>
+      </c>
+      <c r="R38" s="9">
+        <v>4.7E-2</v>
+      </c>
+      <c r="S38" s="9">
+        <v>0.995</v>
+      </c>
+      <c r="T38" s="9">
+        <v>0.746</v>
+      </c>
+      <c r="U38" s="9">
+        <v>0.39500000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="A39" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C39" s="15">
+        <v>7</v>
+      </c>
+      <c r="D39" s="13">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="E39" s="13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="F39" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G39" s="9">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="H39" s="9">
+        <v>1.6E-2</v>
+      </c>
+      <c r="I39" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J39" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="K39" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L39" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M39" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N39" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O39" s="13">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="P39" s="9">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="Q39" s="9">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="R39" s="9">
+        <v>0.115</v>
+      </c>
+      <c r="S39" s="9">
+        <v>0.995</v>
+      </c>
+      <c r="T39" s="9">
+        <v>0.746</v>
+      </c>
+      <c r="U39" s="9">
+        <v>0.39500000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
+      <c r="A40" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="15">
+        <v>6</v>
+      </c>
+      <c r="D40" s="13">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="E40" s="13">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="F40" s="13">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="G40" s="9">
+        <v>0.106</v>
+      </c>
+      <c r="H40" s="9">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="I40" s="9">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="J40" s="9">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="K40" s="9">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="L40" s="9">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="M40" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N40" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O40" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="P40" s="12">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="Q40" s="12">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="R40" s="12">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="S40" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T40" s="9">
+        <v>0.999</v>
+      </c>
+      <c r="U40" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
+      <c r="A41" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="15">
+        <v>5</v>
+      </c>
+      <c r="D41" s="13">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E41" s="13">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F41" s="13">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="G41" s="9">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="H41" s="9">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I41" s="9">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J41" s="9">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="K41" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="L41" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M41" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N41" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O41" s="13">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="P41" s="9">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="Q41" s="9">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="R41" s="9">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="S41" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T41" s="9">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="U41" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21">
+      <c r="A42" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="15">
+        <v>5</v>
+      </c>
+      <c r="D42" s="13">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E42" s="13">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F42" s="13">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="G42" s="9">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="H42" s="9">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="I42" s="9">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J42" s="9">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="K42" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="L42" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M42" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N42" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O42" s="13">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="P42" s="9">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="Q42" s="9">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="R42" s="9">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="S42" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T42" s="9">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="U42" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
+      <c r="A43" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C43" s="15">
+        <v>7</v>
+      </c>
+      <c r="D43" s="13">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="E43" s="13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="F43" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G43" s="9">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H43" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I43" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="J43" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="K43" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L43" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M43" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N43" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O43" s="13">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="P43" s="9">
+        <v>0.33</v>
+      </c>
+      <c r="Q43" s="9">
+        <v>0.161</v>
+      </c>
+      <c r="R43" s="9">
+        <v>4.7E-2</v>
+      </c>
+      <c r="S43" s="9">
+        <v>0.995</v>
+      </c>
+      <c r="T43" s="9">
+        <v>0.746</v>
+      </c>
+      <c r="U43" s="9">
+        <v>0.39500000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
+      <c r="A44" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="15">
+        <v>3</v>
+      </c>
+      <c r="D44" s="13">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="E44" s="13">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="F44" s="13">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="G44" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="H44" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="I44" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="J44" s="9">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="K44" s="9">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="L44" s="9">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="M44" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N44" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O44" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="P44" s="9">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="Q44" s="9">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="R44" s="9">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="S44" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T44" s="9">
+        <v>0.996</v>
+      </c>
+      <c r="U44" s="9">
+        <v>0.82299999999999995</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
+      <c r="A45" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" s="15">
+        <v>5</v>
+      </c>
+      <c r="D45" s="13">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E45" s="13">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F45" s="13">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="G45" s="9">
+        <v>6.3E-2</v>
+      </c>
+      <c r="H45" s="9">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="I45" s="9">
+        <v>1.2E-2</v>
+      </c>
+      <c r="J45" s="9">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="K45" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="L45" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M45" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N45" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O45" s="13">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="P45" s="9">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="Q45" s="9">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="R45" s="9">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="S45" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T45" s="9">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="U45" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21">
+      <c r="A46" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C46" s="15">
+        <v>7</v>
+      </c>
+      <c r="D46" s="13">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="E46" s="13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="F46" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G46" s="9">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="H46" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I46" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="J46" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="K46" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L46" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M46" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N46" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O46" s="13">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="P46" s="9">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="Q46" s="9">
+        <v>0.127</v>
+      </c>
+      <c r="R46" s="9">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="S46" s="9">
+        <v>0.995</v>
+      </c>
+      <c r="T46" s="9">
+        <v>0.746</v>
+      </c>
+      <c r="U46" s="9">
+        <v>0.39500000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21">
+      <c r="A47" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47" s="15">
+        <v>7</v>
+      </c>
+      <c r="D47" s="13">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="E47" s="13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="F47" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G47" s="9">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="H47" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="I47" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J47" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="K47" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L47" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M47" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N47" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O47" s="13">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="P47" s="9">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="Q47" s="9">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="R47" s="9">
+        <v>0.129</v>
+      </c>
+      <c r="S47" s="9">
+        <v>0.995</v>
+      </c>
+      <c r="T47" s="9">
+        <v>0.746</v>
+      </c>
+      <c r="U47" s="9">
+        <v>0.39500000000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
+      <c r="A48" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C48" s="15">
+        <v>7</v>
+      </c>
+      <c r="D48" s="13">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="E48" s="13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="F48" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G48" s="9">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="H48" s="9">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I48" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J48" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="K48" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L48" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M48" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N48" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O48" s="13">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="P48" s="9">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="Q48" s="9">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="R48" s="9">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="S48" s="9">
+        <v>0.995</v>
+      </c>
+      <c r="T48" s="9">
+        <v>0.746</v>
+      </c>
+      <c r="U48" s="9">
+        <v>0.39500000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21">
+      <c r="A49" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" s="15">
+        <v>4</v>
+      </c>
+      <c r="D49" s="11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E49" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F49" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G49" s="9">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="H49" s="9">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="I49" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J49" s="9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K49" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="L49" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M49" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N49" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O49" s="13">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P49" s="9">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="Q49" s="9">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="R49" s="9">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="S49" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T49" s="9">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U49" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21">
+      <c r="A50" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="15">
+        <v>7</v>
+      </c>
+      <c r="D50" s="13">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="E50" s="13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="F50" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G50" s="9">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="H50" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="I50" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J50" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="K50" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L50" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M50" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N50" s="13">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="O50" s="13">
+        <v>0.69699999999999995</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21">
+      <c r="A51" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" s="15">
+        <v>4</v>
+      </c>
+      <c r="D51" s="11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E51" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F51" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G51" s="9">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="H51" s="9">
+        <v>1.9E-2</v>
+      </c>
+      <c r="I51" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="J51" s="9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K51" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="L51" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M51" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N51" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O51" s="13">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P51" s="9">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="Q51" s="9">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="R51" s="9">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="S51" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T51" s="9">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U51" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21">
+      <c r="A52" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="15">
+        <v>3</v>
+      </c>
+      <c r="D52" s="13">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="E52" s="13">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="F52" s="13">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="G52" s="9">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="H52" s="9">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="I52" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="J52" s="9">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="K52" s="9">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="L52" s="9">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="M52" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N52" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O52" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="P52" s="9">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="Q52" s="9">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="R52" s="9">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="S52" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T52" s="9">
+        <v>0.996</v>
+      </c>
+      <c r="U52" s="9">
+        <v>0.82299999999999995</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21">
+      <c r="A53" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" s="15">
+        <v>4</v>
+      </c>
+      <c r="D53" s="11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E53" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F53" s="11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G53" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="H53" s="9">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="I53" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="J53" s="9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="K53" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="L53" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="M53" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N53" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O53" s="13">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="P53" s="9">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="Q53" s="9">
+        <v>0.438</v>
+      </c>
+      <c r="R53" s="9">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="S53" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="T53" s="9">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="U53" s="9">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21">
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="M54" s="13"/>
+      <c r="N54" s="13"/>
+      <c r="O54" s="13"/>
+    </row>
+    <row r="55" spans="1:21">
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="M55" s="13"/>
+      <c r="N55" s="13"/>
+      <c r="O55" s="13"/>
+    </row>
+    <row r="56" spans="1:21">
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="M56" s="13"/>
+      <c r="N56" s="13"/>
+      <c r="O56" s="13"/>
+    </row>
+    <row r="57" spans="1:21">
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="M57" s="13"/>
+      <c r="N57" s="13"/>
+      <c r="O57" s="13"/>
+    </row>
+    <row r="58" spans="1:21">
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="M58" s="13"/>
+      <c r="N58" s="13"/>
+      <c r="O58" s="13"/>
+    </row>
+    <row r="59" spans="1:21">
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="M59" s="13"/>
+      <c r="N59" s="13"/>
+      <c r="O59" s="13"/>
+    </row>
+    <row r="60" spans="1:21">
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="M60" s="13"/>
+      <c r="N60" s="13"/>
+      <c r="O60" s="13"/>
+    </row>
+    <row r="61" spans="1:21">
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="M61" s="13"/>
+      <c r="N61" s="13"/>
+      <c r="O61" s="13"/>
+    </row>
+    <row r="62" spans="1:21">
+      <c r="M62" s="13"/>
+      <c r="N62" s="13"/>
+      <c r="O62" s="13"/>
+    </row>
+    <row r="63" spans="1:21">
+      <c r="M63" s="13"/>
+      <c r="N63" s="13"/>
+      <c r="O63" s="13"/>
+    </row>
+    <row r="1048575" spans="13:13">
+      <c r="M1048575" s="12"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A3:U53" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="3" width="8.7265625" style="10"/>
-    <col min="4" max="4" width="16" style="10" customWidth="1"/>
-    <col min="5" max="5" width="13.36328125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="15" style="10" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" style="10" customWidth="1"/>
-    <col min="8" max="8" width="13.08984375" style="10" customWidth="1"/>
-    <col min="9" max="9" width="20.08984375" style="10" customWidth="1"/>
-    <col min="10" max="10" width="12.90625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="16.6328125" style="10" customWidth="1"/>
-    <col min="12" max="12" width="19.36328125" style="10" customWidth="1"/>
-    <col min="13" max="13" width="15.36328125" style="10" customWidth="1"/>
-    <col min="14" max="14" width="15.08984375" style="10" customWidth="1"/>
-    <col min="15" max="15" width="16.90625" style="10" customWidth="1"/>
-    <col min="16" max="16" width="18.08984375" style="10" customWidth="1"/>
-    <col min="17" max="17" width="14.453125" style="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.7265625" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.90625" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.08984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.7265625" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="9"/>
-      <c r="D2" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="R3" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="T3" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="U3" s="13" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="10">
-        <v>4</v>
-      </c>
-      <c r="D4" s="11">
-        <v>0.47099999999999997</v>
-      </c>
-      <c r="E4" s="12">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="F4" s="12">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="G4" s="12">
-        <v>0.104</v>
-      </c>
-      <c r="H4" s="12">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="I4" s="12">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="J4" s="12">
-        <v>0.36499999999999999</v>
-      </c>
-      <c r="K4" s="12">
-        <v>0.113</v>
-      </c>
-      <c r="L4" s="12">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="O4" s="12">
-        <v>0.54800000000000004</v>
-      </c>
-      <c r="P4" s="12">
-        <v>0.95399999999999996</v>
-      </c>
-      <c r="Q4" s="12">
-        <v>0.73</v>
-      </c>
-      <c r="R4" s="12">
-        <v>0.127</v>
-      </c>
-      <c r="S4" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="T4" s="12">
-        <v>0.96499999999999997</v>
-      </c>
-      <c r="U4" s="12">
-        <v>0.55400000000000005</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated landfall by county
</commit_message>
<xml_diff>
--- a/Project -BH/landfall_probabilities.xlsx
+++ b/Project -BH/landfall_probabilities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12038\Project-1-\Project -BH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163E06DA-E313-4B12-B9BA-1B561040CC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBAB131-A1D6-4685-B9D9-9DA55AB77CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -618,7 +618,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -1147,14 +1147,14 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="21" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="20" fillId="33" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="21" fillId="33" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="20" fillId="33" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="20" fillId="33" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="21" fillId="33" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="20" fillId="33" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1566,7 +1566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M113"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -5654,7 +5654,7 @@
   <dimension ref="A1:U1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -8805,6 +8805,24 @@
       <c r="O50" s="13">
         <v>0.69699999999999995</v>
       </c>
+      <c r="P50" s="9">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="Q50" s="9">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="R50" s="9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="S50" s="9">
+        <v>0.995</v>
+      </c>
+      <c r="T50" s="9">
+        <v>0.746</v>
+      </c>
+      <c r="U50" s="9">
+        <v>0.39500000000000002</v>
+      </c>
     </row>
     <row r="51" spans="1:21">
       <c r="A51" s="9" t="s">

</xml_diff>